<commit_message>
Initial beta version 0.2
This version already contains the final data for a 1.0 release.
</commit_message>
<xml_diff>
--- a/doc/Cisco IP Phone-resolution-matrix.xlsx
+++ b/doc/Cisco IP Phone-resolution-matrix.xlsx
@@ -1267,7 +1267,7 @@
     <t>800x480x24</t>
   </si>
   <si>
-    <t>640x380x24</t>
+    <t>640x480x24</t>
   </si>
 </sst>
 </file>
@@ -1342,8 +1342,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1464,12 +1466,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1527,6 +1529,7 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1584,6 +1587,7 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1931,7 +1935,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H32"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1953,12 +1957,12 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
@@ -1979,10 +1983,10 @@
       <c r="D2">
         <v>4</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>7942</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>7962</v>
       </c>
       <c r="K2" t="s">
@@ -2003,10 +2007,10 @@
       <c r="D3">
         <v>12</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>7970</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>7971</v>
       </c>
       <c r="K3" t="s">
@@ -2027,10 +2031,10 @@
       <c r="D4">
         <v>16</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>7945</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>7965</v>
       </c>
       <c r="K4" t="s">
@@ -2051,7 +2055,7 @@
       <c r="D5">
         <v>16</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>7975</v>
       </c>
       <c r="K5" t="s">
@@ -2072,19 +2076,19 @@
       <c r="D6">
         <v>24</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>8941</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>8945</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>8961</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>9951</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>9971</v>
       </c>
       <c r="K6" t="s">
@@ -2105,7 +2109,7 @@
       <c r="D7">
         <v>16</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>7985</v>
       </c>
       <c r="K7" t="s">
@@ -2126,16 +2130,16 @@
       <c r="D8">
         <v>24</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>8811</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>8841</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>8851</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>8861</v>
       </c>
       <c r="K8" t="s">
@@ -2156,10 +2160,10 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>7906</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>7911</v>
       </c>
       <c r="K9" t="s">
@@ -2408,7 +2412,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v>586 =&gt; {model =&gt;'8941', res =&gt;'640x380x24'},</v>
+        <v>586 =&gt; {model =&gt;'8941', res =&gt;'640x480x24'},</v>
       </c>
     </row>
     <row r="29" spans="2:8">
@@ -2423,7 +2427,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v>585 =&gt; {model =&gt;'8945', res =&gt;'640x380x24'},</v>
+        <v>585 =&gt; {model =&gt;'8945', res =&gt;'640x480x24'},</v>
       </c>
     </row>
     <row r="30" spans="2:8">
@@ -2438,7 +2442,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
-        <v>540 =&gt; {model =&gt;'8961', res =&gt;'640x380x24'},</v>
+        <v>540 =&gt; {model =&gt;'8961', res =&gt;'640x480x24'},</v>
       </c>
     </row>
     <row r="31" spans="2:8">
@@ -2453,7 +2457,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
-        <v>537 =&gt; {model =&gt;'9951', res =&gt;'640x380x24'},</v>
+        <v>537 =&gt; {model =&gt;'9951', res =&gt;'640x480x24'},</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -2468,7 +2472,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
-        <v>493 =&gt; {model =&gt;'9971', res =&gt;'640x380x24'},</v>
+        <v>493 =&gt; {model =&gt;'9971', res =&gt;'640x480x24'},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create template in XLS for documentation in Wiki
</commit_message>
<xml_diff>
--- a/doc/Cisco IP Phone-resolution-matrix.xlsx
+++ b/doc/Cisco IP Phone-resolution-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="2800" windowWidth="37860" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="6060" yWindow="4420" windowWidth="37860" windowHeight="17400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1342,8 +1342,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1471,7 +1491,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1530,6 +1550,16 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1588,6 +1618,16 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1932,10 +1972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1944,7 +1984,7 @@
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +2009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>320</v>
       </c>
@@ -1993,7 +2033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>320</v>
       </c>
@@ -2017,7 +2057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>320</v>
       </c>
@@ -2041,7 +2081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>320</v>
       </c>
@@ -2062,7 +2102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>640</v>
       </c>
@@ -2095,7 +2135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>800</v>
       </c>
@@ -2116,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>800</v>
       </c>
@@ -2146,7 +2186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>95</v>
       </c>
@@ -2170,7 +2210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3264</v>
       </c>
@@ -2182,7 +2222,7 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="B13" t="s">
         <v>398</v>
       </c>
@@ -2190,7 +2230,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="B14">
         <v>7906</v>
       </c>
@@ -2204,8 +2244,12 @@
         <f>D14&amp;" =&gt; {model =&gt;'"&amp;B14&amp;"', res =&gt;'"&amp;E14&amp;"'},"</f>
         <v>369 =&gt; {model =&gt;'7906', res =&gt;'95x34x1'},</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="M14" t="str">
+        <f>"| "&amp;B14&amp; "|| "&amp; D14&amp;" || &lt;tt&gt;"&amp;E14&amp;"&lt;/tt&gt;"</f>
+        <v>| 7906|| 369 || &lt;tt&gt;95x34x1&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="B15">
         <v>7911</v>
       </c>
@@ -2219,8 +2263,12 @@
         <f t="shared" ref="H15:H32" si="1">D15&amp;" =&gt; {model =&gt;'"&amp;B15&amp;"', res =&gt;'"&amp;E15&amp;"'},"</f>
         <v>307 =&gt; {model =&gt;'7911', res =&gt;'95x34x1'},</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="M15" t="str">
+        <f t="shared" ref="M15:M32" si="2">"| "&amp;B15&amp; "|| "&amp; D15&amp;" || &lt;tt&gt;"&amp;E15&amp;"&lt;/tt&gt;"</f>
+        <v>| 7911|| 307 || &lt;tt&gt;95x34x1&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="B16">
         <v>7942</v>
       </c>
@@ -2234,8 +2282,12 @@
         <f t="shared" si="1"/>
         <v>434 =&gt; {model =&gt;'7942', res =&gt;'320x196x4'},</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="M16" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7942|| 434 || &lt;tt&gt;320x196x4&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17">
         <v>7945</v>
       </c>
@@ -2249,8 +2301,12 @@
         <f t="shared" si="1"/>
         <v>435 =&gt; {model =&gt;'7945', res =&gt;'320x212x16'},</v>
       </c>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="M17" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7945|| 435 || &lt;tt&gt;320x212x16&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18">
         <v>7962</v>
       </c>
@@ -2264,8 +2320,12 @@
         <f t="shared" si="1"/>
         <v>404 =&gt; {model =&gt;'7962', res =&gt;'320x212x16'},</v>
       </c>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="M18" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7962|| 404 || &lt;tt&gt;320x212x16&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19">
         <v>7965</v>
       </c>
@@ -2279,8 +2339,12 @@
         <f t="shared" si="1"/>
         <v>436 =&gt; {model =&gt;'7965', res =&gt;'320x196x4'},</v>
       </c>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="M19" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7965|| 436 || &lt;tt&gt;320x196x4&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20">
         <v>7970</v>
       </c>
@@ -2294,8 +2358,12 @@
         <f t="shared" si="1"/>
         <v>30006 =&gt; {model =&gt;'7970', res =&gt;'320x212x12'},</v>
       </c>
-    </row>
-    <row r="21" spans="2:8">
+      <c r="M20" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7970|| 30006 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21">
         <v>7971</v>
       </c>
@@ -2309,8 +2377,12 @@
         <f t="shared" si="1"/>
         <v>119 =&gt; {model =&gt;'7971', res =&gt;'320x212x12'},</v>
       </c>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="M21" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7971|| 119 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22">
         <v>7975</v>
       </c>
@@ -2324,8 +2396,12 @@
         <f t="shared" si="1"/>
         <v>437 =&gt; {model =&gt;'7975', res =&gt;'320x216x16'},</v>
       </c>
-    </row>
-    <row r="23" spans="2:8">
+      <c r="M22" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7975|| 437 || &lt;tt&gt;320x216x16&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
       <c r="B23">
         <v>7985</v>
       </c>
@@ -2339,8 +2415,12 @@
         <f t="shared" si="1"/>
         <v>302 =&gt; {model =&gt;'7985', res =&gt;'800x600x16'},</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="M23" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7985|| 302 || &lt;tt&gt;800x600x16&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
       <c r="B24">
         <v>8811</v>
       </c>
@@ -2354,8 +2434,12 @@
         <f t="shared" si="1"/>
         <v>36217 =&gt; {model =&gt;'8811', res =&gt;'800x480x24'},</v>
       </c>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="M24" t="str">
+        <f t="shared" si="2"/>
+        <v>| 8811|| 36217 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
       <c r="B25">
         <v>8841</v>
       </c>
@@ -2369,8 +2453,12 @@
         <f t="shared" si="1"/>
         <v>683 =&gt; {model =&gt;'8841', res =&gt;'800x480x24'},</v>
       </c>
-    </row>
-    <row r="26" spans="2:8">
+      <c r="M25" t="str">
+        <f t="shared" si="2"/>
+        <v>| 8841|| 683 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
       <c r="B26">
         <v>8851</v>
       </c>
@@ -2384,8 +2472,12 @@
         <f t="shared" si="1"/>
         <v>684 =&gt; {model =&gt;'8851', res =&gt;'800x480x24'},</v>
       </c>
-    </row>
-    <row r="27" spans="2:8">
+      <c r="M26" t="str">
+        <f t="shared" si="2"/>
+        <v>| 8851|| 684 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
       <c r="B27">
         <v>8861</v>
       </c>
@@ -2399,8 +2491,12 @@
         <f t="shared" si="1"/>
         <v>685 =&gt; {model =&gt;'8861', res =&gt;'800x480x24'},</v>
       </c>
-    </row>
-    <row r="28" spans="2:8">
+      <c r="M27" t="str">
+        <f t="shared" si="2"/>
+        <v>| 8861|| 685 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
       <c r="B28">
         <v>8941</v>
       </c>
@@ -2414,8 +2510,12 @@
         <f t="shared" si="1"/>
         <v>586 =&gt; {model =&gt;'8941', res =&gt;'640x480x24'},</v>
       </c>
-    </row>
-    <row r="29" spans="2:8">
+      <c r="M28" t="str">
+        <f t="shared" si="2"/>
+        <v>| 8941|| 586 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29">
         <v>8945</v>
       </c>
@@ -2429,8 +2529,12 @@
         <f t="shared" si="1"/>
         <v>585 =&gt; {model =&gt;'8945', res =&gt;'640x480x24'},</v>
       </c>
-    </row>
-    <row r="30" spans="2:8">
+      <c r="M29" t="str">
+        <f t="shared" si="2"/>
+        <v>| 8945|| 585 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
       <c r="B30">
         <v>8961</v>
       </c>
@@ -2444,8 +2548,12 @@
         <f t="shared" si="1"/>
         <v>540 =&gt; {model =&gt;'8961', res =&gt;'640x480x24'},</v>
       </c>
-    </row>
-    <row r="31" spans="2:8">
+      <c r="M30" t="str">
+        <f t="shared" si="2"/>
+        <v>| 8961|| 540 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
       <c r="B31">
         <v>9951</v>
       </c>
@@ -2459,8 +2567,12 @@
         <f t="shared" si="1"/>
         <v>537 =&gt; {model =&gt;'9951', res =&gt;'640x480x24'},</v>
       </c>
-    </row>
-    <row r="32" spans="2:8">
+      <c r="M31" t="str">
+        <f t="shared" si="2"/>
+        <v>| 9951|| 537 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32">
         <v>9971</v>
       </c>
@@ -2473,6 +2585,10 @@
       <c r="H32" t="str">
         <f t="shared" si="1"/>
         <v>493 =&gt; {model =&gt;'9971', res =&gt;'640x480x24'},</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="2"/>
+        <v>| 9971|| 493 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected 88/89XX series thumbnail sizes
</commit_message>
<xml_diff>
--- a/doc/Cisco IP Phone-resolution-matrix.xlsx
+++ b/doc/Cisco IP Phone-resolution-matrix.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\pbp\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="4420" windowWidth="37860" windowHeight="17400" tabRatio="500"/>
+    <workbookView xWindow="6060" yWindow="4425" windowWidth="37860" windowHeight="17400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CUCM 10.5 DB'!$A$1:$I$188</definedName>
     <definedName name="cucm_phone_models" localSheetId="1">'CUCM 10.5 DB'!$A$1:$I$188</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -44,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="417">
   <si>
     <t>Width</t>
   </si>
@@ -1268,13 +1273,40 @@
   </si>
   <si>
     <t>640x480x24</t>
+  </si>
+  <si>
+    <t>Thumbnail</t>
+  </si>
+  <si>
+    <t>80x49</t>
+  </si>
+  <si>
+    <t>80x53</t>
+  </si>
+  <si>
+    <t>123x11</t>
+  </si>
+  <si>
+    <t>No thumbnail</t>
+  </si>
+  <si>
+    <t>159x109</t>
+  </si>
+  <si>
+    <t>23x8</t>
+  </si>
+  <si>
+    <t>Perl hash entries</t>
+  </si>
+  <si>
+    <t>Wiki table entry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1306,6 +1338,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1333,9 +1371,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -1481,7 +1528,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1490,6 +1537,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1643,6 +1696,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1972,19 +2033,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1995,599 +2058,751 @@
         <v>399</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="1"/>
+      <c r="I1" s="5"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>320</v>
       </c>
       <c r="B2">
         <v>196</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <f>A2/B2</f>
         <v>1.6326530612244898</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>7942</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>7962</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>320</v>
       </c>
       <c r="B3">
         <v>212</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="7">
         <f t="shared" ref="C3:C10" si="0">A3/B3</f>
         <v>1.5094339622641511</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="E3">
         <v>12</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>7970</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>7971</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>320</v>
       </c>
       <c r="B4">
         <v>212</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="7">
         <f t="shared" si="0"/>
         <v>1.5094339622641511</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="E4">
         <v>16</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>7945</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>7965</v>
       </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>320</v>
       </c>
       <c r="B5">
         <v>216</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>1.4814814814814814</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>410</v>
+      </c>
+      <c r="E5">
         <v>16</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>7975</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>640</v>
       </c>
       <c r="B6">
         <v>480</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="8">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E6">
         <v>24</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>8941</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>8945</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>8961</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>9951</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>9971</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>800</v>
       </c>
       <c r="B7">
         <v>600</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E7">
         <v>16</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>7985</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>800</v>
       </c>
       <c r="B8">
         <v>480</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>413</v>
+      </c>
+      <c r="E8">
         <v>24</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="4">
         <v>8811</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>8841</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>8851</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>8861</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>95</v>
       </c>
       <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>2.7941176470588234</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
         <v>7906</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>7911</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3264</v>
       </c>
       <c r="B10">
         <v>2448</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="B13" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="1" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>7906</v>
       </c>
-      <c r="D14">
+      <c r="C14">
         <v>369</v>
       </c>
+      <c r="D14" t="s">
+        <v>400</v>
+      </c>
       <c r="E14" t="s">
-        <v>400</v>
-      </c>
-      <c r="H14" t="str">
-        <f>D14&amp;" =&gt; {model =&gt;'"&amp;B14&amp;"', res =&gt;'"&amp;E14&amp;"'},"</f>
+        <v>414</v>
+      </c>
+      <c r="G14" s="10" t="str">
+        <f>C14&amp;" =&gt; {model =&gt;'"&amp;B14&amp;"', res =&gt;'"&amp;D14&amp;"'},"</f>
         <v>369 =&gt; {model =&gt;'7906', res =&gt;'95x34x1'},</v>
       </c>
-      <c r="M14" t="str">
-        <f>"| "&amp;B14&amp; "|| "&amp; D14&amp;" || &lt;tt&gt;"&amp;E14&amp;"&lt;/tt&gt;"</f>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="L14" s="11" t="str">
+        <f>"| "&amp;B14&amp; "|| "&amp; C14&amp;" || &lt;tt&gt;"&amp;D14&amp;"&lt;/tt&gt;"</f>
         <v>| 7906|| 369 || &lt;tt&gt;95x34x1&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>7911</v>
       </c>
-      <c r="D15">
+      <c r="C15">
         <v>307</v>
       </c>
+      <c r="D15" t="s">
+        <v>400</v>
+      </c>
       <c r="E15" t="s">
-        <v>400</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" ref="H15:H32" si="1">D15&amp;" =&gt; {model =&gt;'"&amp;B15&amp;"', res =&gt;'"&amp;E15&amp;"'},"</f>
+        <v>414</v>
+      </c>
+      <c r="G15" s="10" t="str">
+        <f>C15&amp;" =&gt; {model =&gt;'"&amp;B15&amp;"', res =&gt;'"&amp;D15&amp;"'},"</f>
         <v>307 =&gt; {model =&gt;'7911', res =&gt;'95x34x1'},</v>
       </c>
-      <c r="M15" t="str">
-        <f t="shared" ref="M15:M32" si="2">"| "&amp;B15&amp; "|| "&amp; D15&amp;" || &lt;tt&gt;"&amp;E15&amp;"&lt;/tt&gt;"</f>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="L15" s="11" t="str">
+        <f>"| "&amp;B15&amp; "|| "&amp; C15&amp;" || &lt;tt&gt;"&amp;D15&amp;"&lt;/tt&gt;"</f>
         <v>| 7911|| 307 || &lt;tt&gt;95x34x1&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>7942</v>
       </c>
-      <c r="D16">
+      <c r="C16">
         <v>434</v>
       </c>
+      <c r="D16" t="s">
+        <v>401</v>
+      </c>
       <c r="E16" t="s">
-        <v>401</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="1"/>
+        <v>409</v>
+      </c>
+      <c r="G16" s="10" t="str">
+        <f>C16&amp;" =&gt; {model =&gt;'"&amp;B16&amp;"', res =&gt;'"&amp;D16&amp;"'},"</f>
         <v>434 =&gt; {model =&gt;'7942', res =&gt;'320x196x4'},</v>
       </c>
-      <c r="M16" t="str">
-        <f t="shared" si="2"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="L16" s="11" t="str">
+        <f>"| "&amp;B16&amp; "|| "&amp; C16&amp;" || &lt;tt&gt;"&amp;D16&amp;"&lt;/tt&gt;"</f>
         <v>| 7942|| 434 || &lt;tt&gt;320x196x4&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>7945</v>
       </c>
-      <c r="D17">
+      <c r="C17">
         <v>435</v>
       </c>
+      <c r="D17" t="s">
+        <v>402</v>
+      </c>
       <c r="E17" t="s">
-        <v>402</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="G17" s="10" t="str">
+        <f>C17&amp;" =&gt; {model =&gt;'"&amp;B17&amp;"', res =&gt;'"&amp;D17&amp;"'},"</f>
         <v>435 =&gt; {model =&gt;'7945', res =&gt;'320x212x16'},</v>
       </c>
-      <c r="M17" t="str">
-        <f t="shared" si="2"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="L17" s="11" t="str">
+        <f>"| "&amp;B17&amp; "|| "&amp; C17&amp;" || &lt;tt&gt;"&amp;D17&amp;"&lt;/tt&gt;"</f>
         <v>| 7945|| 435 || &lt;tt&gt;320x212x16&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>7962</v>
       </c>
-      <c r="D18">
+      <c r="C18">
         <v>404</v>
       </c>
+      <c r="D18" t="s">
+        <v>402</v>
+      </c>
       <c r="E18" t="s">
-        <v>402</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="G18" s="10" t="str">
+        <f>C18&amp;" =&gt; {model =&gt;'"&amp;B18&amp;"', res =&gt;'"&amp;D18&amp;"'},"</f>
         <v>404 =&gt; {model =&gt;'7962', res =&gt;'320x212x16'},</v>
       </c>
-      <c r="M18" t="str">
-        <f t="shared" si="2"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="L18" s="11" t="str">
+        <f>"| "&amp;B18&amp; "|| "&amp; C18&amp;" || &lt;tt&gt;"&amp;D18&amp;"&lt;/tt&gt;"</f>
         <v>| 7962|| 404 || &lt;tt&gt;320x212x16&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>7965</v>
       </c>
-      <c r="D19">
+      <c r="C19">
         <v>436</v>
       </c>
+      <c r="D19" t="s">
+        <v>401</v>
+      </c>
       <c r="E19" t="s">
-        <v>401</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="G19" s="10" t="str">
+        <f>C19&amp;" =&gt; {model =&gt;'"&amp;B19&amp;"', res =&gt;'"&amp;D19&amp;"'},"</f>
         <v>436 =&gt; {model =&gt;'7965', res =&gt;'320x196x4'},</v>
       </c>
-      <c r="M19" t="str">
-        <f t="shared" si="2"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="L19" s="11" t="str">
+        <f>"| "&amp;B19&amp; "|| "&amp; C19&amp;" || &lt;tt&gt;"&amp;D19&amp;"&lt;/tt&gt;"</f>
         <v>| 7965|| 436 || &lt;tt&gt;320x196x4&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>7970</v>
       </c>
-      <c r="D20">
+      <c r="C20">
         <v>30006</v>
       </c>
+      <c r="D20" t="s">
+        <v>403</v>
+      </c>
       <c r="E20" t="s">
-        <v>403</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="G20" s="10" t="str">
+        <f>C20&amp;" =&gt; {model =&gt;'"&amp;B20&amp;"', res =&gt;'"&amp;D20&amp;"'},"</f>
         <v>30006 =&gt; {model =&gt;'7970', res =&gt;'320x212x12'},</v>
       </c>
-      <c r="M20" t="str">
-        <f t="shared" si="2"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="L20" s="11" t="str">
+        <f>"| "&amp;B20&amp; "|| "&amp; C20&amp;" || &lt;tt&gt;"&amp;D20&amp;"&lt;/tt&gt;"</f>
         <v>| 7970|| 30006 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>7971</v>
       </c>
-      <c r="D21">
+      <c r="C21">
         <v>119</v>
       </c>
+      <c r="D21" t="s">
+        <v>403</v>
+      </c>
       <c r="E21" t="s">
-        <v>403</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="G21" s="10" t="str">
+        <f>C21&amp;" =&gt; {model =&gt;'"&amp;B21&amp;"', res =&gt;'"&amp;D21&amp;"'},"</f>
         <v>119 =&gt; {model =&gt;'7971', res =&gt;'320x212x12'},</v>
       </c>
-      <c r="M21" t="str">
-        <f t="shared" si="2"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="L21" s="11" t="str">
+        <f>"| "&amp;B21&amp; "|| "&amp; C21&amp;" || &lt;tt&gt;"&amp;D21&amp;"&lt;/tt&gt;"</f>
         <v>| 7971|| 119 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>7975</v>
       </c>
-      <c r="D22">
+      <c r="C22">
         <v>437</v>
       </c>
+      <c r="D22" t="s">
+        <v>404</v>
+      </c>
       <c r="E22" t="s">
-        <v>404</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="G22" s="10" t="str">
+        <f>C22&amp;" =&gt; {model =&gt;'"&amp;B22&amp;"', res =&gt;'"&amp;D22&amp;"'},"</f>
         <v>437 =&gt; {model =&gt;'7975', res =&gt;'320x216x16'},</v>
       </c>
-      <c r="M22" t="str">
-        <f t="shared" si="2"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="L22" s="11" t="str">
+        <f>"| "&amp;B22&amp; "|| "&amp; C22&amp;" || &lt;tt&gt;"&amp;D22&amp;"&lt;/tt&gt;"</f>
         <v>| 7975|| 437 || &lt;tt&gt;320x216x16&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>7985</v>
       </c>
-      <c r="D23">
+      <c r="C23">
         <v>302</v>
       </c>
+      <c r="D23" t="s">
+        <v>405</v>
+      </c>
       <c r="E23" t="s">
-        <v>405</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="1"/>
+        <v>412</v>
+      </c>
+      <c r="G23" s="10" t="str">
+        <f>C23&amp;" =&gt; {model =&gt;'"&amp;B23&amp;"', res =&gt;'"&amp;D23&amp;"'},"</f>
         <v>302 =&gt; {model =&gt;'7985', res =&gt;'800x600x16'},</v>
       </c>
-      <c r="M23" t="str">
-        <f t="shared" si="2"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="L23" s="11" t="str">
+        <f>"| "&amp;B23&amp; "|| "&amp; C23&amp;" || &lt;tt&gt;"&amp;D23&amp;"&lt;/tt&gt;"</f>
         <v>| 7985|| 302 || &lt;tt&gt;800x600x16&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>8811</v>
       </c>
-      <c r="D24">
+      <c r="C24">
         <v>36217</v>
       </c>
+      <c r="D24" t="s">
+        <v>406</v>
+      </c>
       <c r="E24" t="s">
-        <v>406</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+      <c r="G24" s="10" t="str">
+        <f>C24&amp;" =&gt; {model =&gt;'"&amp;B24&amp;"', res =&gt;'"&amp;D24&amp;"'},"</f>
         <v>36217 =&gt; {model =&gt;'8811', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="M24" t="str">
-        <f t="shared" si="2"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="L24" s="11" t="str">
+        <f>"| "&amp;B24&amp; "|| "&amp; C24&amp;" || &lt;tt&gt;"&amp;D24&amp;"&lt;/tt&gt;"</f>
         <v>| 8811|| 36217 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>8841</v>
       </c>
-      <c r="D25">
+      <c r="C25">
         <v>683</v>
       </c>
+      <c r="D25" t="s">
+        <v>406</v>
+      </c>
       <c r="E25" t="s">
-        <v>406</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+      <c r="G25" s="10" t="str">
+        <f>C25&amp;" =&gt; {model =&gt;'"&amp;B25&amp;"', res =&gt;'"&amp;D25&amp;"'},"</f>
         <v>683 =&gt; {model =&gt;'8841', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="M25" t="str">
-        <f t="shared" si="2"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="L25" s="11" t="str">
+        <f>"| "&amp;B25&amp; "|| "&amp; C25&amp;" || &lt;tt&gt;"&amp;D25&amp;"&lt;/tt&gt;"</f>
         <v>| 8841|| 683 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>8851</v>
       </c>
-      <c r="D26">
+      <c r="C26">
         <v>684</v>
       </c>
+      <c r="D26" t="s">
+        <v>406</v>
+      </c>
       <c r="E26" t="s">
-        <v>406</v>
-      </c>
-      <c r="H26" t="str">
-        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+      <c r="G26" s="10" t="str">
+        <f>C26&amp;" =&gt; {model =&gt;'"&amp;B26&amp;"', res =&gt;'"&amp;D26&amp;"'},"</f>
         <v>684 =&gt; {model =&gt;'8851', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="M26" t="str">
-        <f t="shared" si="2"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="L26" s="11" t="str">
+        <f>"| "&amp;B26&amp; "|| "&amp; C26&amp;" || &lt;tt&gt;"&amp;D26&amp;"&lt;/tt&gt;"</f>
         <v>| 8851|| 684 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>8861</v>
       </c>
-      <c r="D27">
+      <c r="C27">
         <v>685</v>
       </c>
+      <c r="D27" t="s">
+        <v>406</v>
+      </c>
       <c r="E27" t="s">
-        <v>406</v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+      <c r="G27" s="10" t="str">
+        <f>C27&amp;" =&gt; {model =&gt;'"&amp;B27&amp;"', res =&gt;'"&amp;D27&amp;"'},"</f>
         <v>685 =&gt; {model =&gt;'8861', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="M27" t="str">
-        <f t="shared" si="2"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="L27" s="11" t="str">
+        <f>"| "&amp;B27&amp; "|| "&amp; C27&amp;" || &lt;tt&gt;"&amp;D27&amp;"&lt;/tt&gt;"</f>
         <v>| 8861|| 685 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>8941</v>
       </c>
-      <c r="D28">
+      <c r="C28">
         <v>586</v>
       </c>
+      <c r="D28" t="s">
+        <v>407</v>
+      </c>
       <c r="E28" t="s">
-        <v>407</v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="G28" s="10" t="str">
+        <f>C28&amp;" =&gt; {model =&gt;'"&amp;B28&amp;"', res =&gt;'"&amp;D28&amp;"'},"</f>
         <v>586 =&gt; {model =&gt;'8941', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="M28" t="str">
-        <f t="shared" si="2"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="L28" s="11" t="str">
+        <f>"| "&amp;B28&amp; "|| "&amp; C28&amp;" || &lt;tt&gt;"&amp;D28&amp;"&lt;/tt&gt;"</f>
         <v>| 8941|| 586 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>8945</v>
       </c>
-      <c r="D29">
+      <c r="C29">
         <v>585</v>
       </c>
+      <c r="D29" t="s">
+        <v>407</v>
+      </c>
       <c r="E29" t="s">
-        <v>407</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="G29" s="10" t="str">
+        <f>C29&amp;" =&gt; {model =&gt;'"&amp;B29&amp;"', res =&gt;'"&amp;D29&amp;"'},"</f>
         <v>585 =&gt; {model =&gt;'8945', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="M29" t="str">
-        <f t="shared" si="2"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="L29" s="11" t="str">
+        <f>"| "&amp;B29&amp; "|| "&amp; C29&amp;" || &lt;tt&gt;"&amp;D29&amp;"&lt;/tt&gt;"</f>
         <v>| 8945|| 585 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>8961</v>
       </c>
-      <c r="D30">
+      <c r="C30">
         <v>540</v>
       </c>
+      <c r="D30" t="s">
+        <v>407</v>
+      </c>
       <c r="E30" t="s">
-        <v>407</v>
-      </c>
-      <c r="H30" t="str">
-        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="G30" s="10" t="str">
+        <f>C30&amp;" =&gt; {model =&gt;'"&amp;B30&amp;"', res =&gt;'"&amp;D30&amp;"'},"</f>
         <v>540 =&gt; {model =&gt;'8961', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="M30" t="str">
-        <f t="shared" si="2"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="L30" s="11" t="str">
+        <f>"| "&amp;B30&amp; "|| "&amp; C30&amp;" || &lt;tt&gt;"&amp;D30&amp;"&lt;/tt&gt;"</f>
         <v>| 8961|| 540 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>9951</v>
       </c>
-      <c r="D31">
+      <c r="C31">
         <v>537</v>
       </c>
+      <c r="D31" t="s">
+        <v>407</v>
+      </c>
       <c r="E31" t="s">
-        <v>407</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="G31" s="10" t="str">
+        <f>C31&amp;" =&gt; {model =&gt;'"&amp;B31&amp;"', res =&gt;'"&amp;D31&amp;"'},"</f>
         <v>537 =&gt; {model =&gt;'9951', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="M31" t="str">
-        <f t="shared" si="2"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="L31" s="11" t="str">
+        <f>"| "&amp;B31&amp; "|| "&amp; C31&amp;" || &lt;tt&gt;"&amp;D31&amp;"&lt;/tt&gt;"</f>
         <v>| 9951|| 537 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>9971</v>
       </c>
-      <c r="D32">
+      <c r="C32">
         <v>493</v>
       </c>
+      <c r="D32" t="s">
+        <v>407</v>
+      </c>
       <c r="E32" t="s">
-        <v>407</v>
-      </c>
-      <c r="H32" t="str">
-        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="G32" s="10" t="str">
+        <f>C32&amp;" =&gt; {model =&gt;'"&amp;B32&amp;"', res =&gt;'"&amp;D32&amp;"'},"</f>
         <v>493 =&gt; {model =&gt;'9971', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="M32" t="str">
-        <f t="shared" si="2"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="L32" s="11" t="str">
+        <f>"| "&amp;B32&amp; "|| "&amp; C32&amp;" || &lt;tt&gt;"&amp;D32&amp;"&lt;/tt&gt;"</f>
         <v>| 9971|| 493 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
@@ -2596,13 +2811,13 @@
     <sortCondition ref="B14"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:I4 E6:I9 H5:I5 E5:F5">
+  <conditionalFormatting sqref="F2:J4 F6:J9 I5:J5 F5:G5">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2619,20 +2834,20 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2661,7 +2876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2690,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2719,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2748,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2777,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2806,7 +3021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2835,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2864,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2893,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2922,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2951,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2980,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3009,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -3038,7 +3253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -3067,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>30</v>
       </c>
@@ -3096,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>40</v>
       </c>
@@ -3125,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>42</v>
       </c>
@@ -3154,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>43</v>
       </c>
@@ -3183,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>47</v>
       </c>
@@ -3212,7 +3427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>48</v>
       </c>
@@ -3241,7 +3456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>50</v>
       </c>
@@ -3270,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>51</v>
       </c>
@@ -3299,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>52</v>
       </c>
@@ -3328,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>53</v>
       </c>
@@ -3357,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>61</v>
       </c>
@@ -3386,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>62</v>
       </c>
@@ -3415,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>70</v>
       </c>
@@ -3444,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>71</v>
       </c>
@@ -3473,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>72</v>
       </c>
@@ -3502,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>73</v>
       </c>
@@ -3531,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>80</v>
       </c>
@@ -3560,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>83</v>
       </c>
@@ -3589,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>84</v>
       </c>
@@ -3618,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>85</v>
       </c>
@@ -3647,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>86</v>
       </c>
@@ -3676,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>87</v>
       </c>
@@ -3705,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>88</v>
       </c>
@@ -3734,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>90</v>
       </c>
@@ -3763,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>100</v>
       </c>
@@ -3792,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>110</v>
       </c>
@@ -3821,7 +4036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>111</v>
       </c>
@@ -3850,7 +4065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>112</v>
       </c>
@@ -3879,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>113</v>
       </c>
@@ -3908,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>115</v>
       </c>
@@ -3937,7 +4152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>119</v>
       </c>
@@ -3966,7 +4181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>120</v>
       </c>
@@ -3995,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>121</v>
       </c>
@@ -4024,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>122</v>
       </c>
@@ -4053,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>124</v>
       </c>
@@ -4082,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>125</v>
       </c>
@@ -4111,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>126</v>
       </c>
@@ -4140,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>131</v>
       </c>
@@ -4169,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>132</v>
       </c>
@@ -4198,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>133</v>
       </c>
@@ -4227,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>134</v>
       </c>
@@ -4256,7 +4471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>227</v>
       </c>
@@ -4285,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>228</v>
       </c>
@@ -4314,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>229</v>
       </c>
@@ -4343,7 +4558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>230</v>
       </c>
@@ -4372,7 +4587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>232</v>
       </c>
@@ -4401,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>253</v>
       </c>
@@ -4430,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>254</v>
       </c>
@@ -4459,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>255</v>
       </c>
@@ -4488,7 +4703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>302</v>
       </c>
@@ -4517,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>307</v>
       </c>
@@ -4546,7 +4761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>308</v>
       </c>
@@ -4575,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>309</v>
       </c>
@@ -4604,7 +4819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>335</v>
       </c>
@@ -4633,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>336</v>
       </c>
@@ -4662,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>348</v>
       </c>
@@ -4691,7 +4906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>358</v>
       </c>
@@ -4720,7 +4935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>365</v>
       </c>
@@ -4749,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>369</v>
       </c>
@@ -4778,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>374</v>
       </c>
@@ -4807,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>375</v>
       </c>
@@ -4836,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>376</v>
       </c>
@@ -4865,7 +5080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>404</v>
       </c>
@@ -4894,7 +5109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>412</v>
       </c>
@@ -4923,7 +5138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>431</v>
       </c>
@@ -4952,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>434</v>
       </c>
@@ -4981,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>435</v>
       </c>
@@ -5010,7 +5225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>436</v>
       </c>
@@ -5039,7 +5254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>437</v>
       </c>
@@ -5068,7 +5283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>446</v>
       </c>
@@ -5097,7 +5312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>468</v>
       </c>
@@ -5126,7 +5341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>478</v>
       </c>
@@ -5155,7 +5370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>479</v>
       </c>
@@ -5184,7 +5399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>480</v>
       </c>
@@ -5213,7 +5428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>481</v>
       </c>
@@ -5242,7 +5457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>484</v>
       </c>
@@ -5271,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>493</v>
       </c>
@@ -5300,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>495</v>
       </c>
@@ -5329,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>496</v>
       </c>
@@ -5358,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>497</v>
       </c>
@@ -5387,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>503</v>
       </c>
@@ -5416,7 +5631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>505</v>
       </c>
@@ -5445,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>520</v>
       </c>
@@ -5474,7 +5689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>521</v>
       </c>
@@ -5503,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>522</v>
       </c>
@@ -5532,7 +5747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>537</v>
       </c>
@@ -5561,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>540</v>
       </c>
@@ -5590,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>547</v>
       </c>
@@ -5619,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>548</v>
       </c>
@@ -5648,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>550</v>
       </c>
@@ -5677,7 +5892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>557</v>
       </c>
@@ -5706,7 +5921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>558</v>
       </c>
@@ -5735,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>562</v>
       </c>
@@ -5764,7 +5979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>564</v>
       </c>
@@ -5793,7 +6008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>575</v>
       </c>
@@ -5822,7 +6037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>577</v>
       </c>
@@ -5851,7 +6066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>580</v>
       </c>
@@ -5880,7 +6095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>582</v>
       </c>
@@ -5909,7 +6124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>583</v>
       </c>
@@ -5938,7 +6153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>584</v>
       </c>
@@ -5967,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>585</v>
       </c>
@@ -5996,7 +6211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>586</v>
       </c>
@@ -6025,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>588</v>
       </c>
@@ -6054,7 +6269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>590</v>
       </c>
@@ -6083,7 +6298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>591</v>
       </c>
@@ -6112,7 +6327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>592</v>
       </c>
@@ -6141,7 +6356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>593</v>
       </c>
@@ -6170,7 +6385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>594</v>
       </c>
@@ -6199,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>596</v>
       </c>
@@ -6228,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>597</v>
       </c>
@@ -6257,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>598</v>
       </c>
@@ -6286,7 +6501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>599</v>
       </c>
@@ -6315,7 +6530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>604</v>
       </c>
@@ -6344,7 +6559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>606</v>
       </c>
@@ -6373,7 +6588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>607</v>
       </c>
@@ -6402,7 +6617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>608</v>
       </c>
@@ -6431,7 +6646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>609</v>
       </c>
@@ -6460,7 +6675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>610</v>
       </c>
@@ -6489,7 +6704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>611</v>
       </c>
@@ -6518,7 +6733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>612</v>
       </c>
@@ -6547,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>613</v>
       </c>
@@ -6576,7 +6791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>614</v>
       </c>
@@ -6605,7 +6820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>615</v>
       </c>
@@ -6634,7 +6849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>616</v>
       </c>
@@ -6663,7 +6878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>617</v>
       </c>
@@ -6692,7 +6907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>619</v>
       </c>
@@ -6721,7 +6936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>620</v>
       </c>
@@ -6750,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>621</v>
       </c>
@@ -6779,7 +6994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>622</v>
       </c>
@@ -6808,7 +7023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>623</v>
       </c>
@@ -6837,7 +7052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>626</v>
       </c>
@@ -6866,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>627</v>
       </c>
@@ -6895,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>628</v>
       </c>
@@ -6924,7 +7139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>631</v>
       </c>
@@ -6953,7 +7168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>632</v>
       </c>
@@ -6982,7 +7197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>633</v>
       </c>
@@ -7011,7 +7226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>634</v>
       </c>
@@ -7040,7 +7255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>635</v>
       </c>
@@ -7069,7 +7284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>640</v>
       </c>
@@ -7098,7 +7313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>642</v>
       </c>
@@ -7127,7 +7342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>645</v>
       </c>
@@ -7156,7 +7371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>647</v>
       </c>
@@ -7185,7 +7400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>648</v>
       </c>
@@ -7214,7 +7429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>652</v>
       </c>
@@ -7243,7 +7458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>659</v>
       </c>
@@ -7272,7 +7487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>681</v>
       </c>
@@ -7301,7 +7516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>682</v>
       </c>
@@ -7330,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>683</v>
       </c>
@@ -7359,7 +7574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>684</v>
       </c>
@@ -7388,7 +7603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>685</v>
       </c>
@@ -7417,7 +7632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>688</v>
       </c>
@@ -7446,7 +7661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>689</v>
       </c>
@@ -7475,7 +7690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>690</v>
       </c>
@@ -7504,7 +7719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>20000</v>
       </c>
@@ -7533,7 +7748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>30002</v>
       </c>
@@ -7562,7 +7777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>30006</v>
       </c>
@@ -7591,7 +7806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>30007</v>
       </c>
@@ -7620,7 +7835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>30008</v>
       </c>
@@ -7649,7 +7864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>30016</v>
       </c>
@@ -7678,7 +7893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>30018</v>
       </c>
@@ -7707,7 +7922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>30019</v>
       </c>
@@ -7736,7 +7951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>30027</v>
       </c>
@@ -7765,7 +7980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>30028</v>
       </c>
@@ -7794,7 +8009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>30032</v>
       </c>
@@ -7823,7 +8038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>30035</v>
       </c>
@@ -7852,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>36041</v>
       </c>
@@ -7881,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>36042</v>
       </c>
@@ -7910,7 +8125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>36043</v>
       </c>
@@ -7939,7 +8154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>36049</v>
       </c>
@@ -7968,7 +8183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>36207</v>
       </c>
@@ -7997,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>36208</v>
       </c>
@@ -8026,7 +8241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>36210</v>
       </c>
@@ -8055,7 +8270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>36217</v>
       </c>

</xml_diff>

<commit_message>
Corrected resolution for 7962 and 7965
The resolution for both models were swapped. Should be corrected now.
</commit_message>
<xml_diff>
--- a/doc/Cisco IP Phone-resolution-matrix.xlsx
+++ b/doc/Cisco IP Phone-resolution-matrix.xlsx
@@ -1306,7 +1306,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1344,6 +1344,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1366,8 +1373,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1389,7 +1395,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1527,24 +1533,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="137"/>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="138">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1613,6 +1620,7 @@
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="137" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2036,7 +2044,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="G14" sqref="G14:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2063,12 +2071,12 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
@@ -2082,7 +2090,7 @@
       <c r="B2">
         <v>196</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="4">
         <f>A2/B2</f>
         <v>1.6326530612244898</v>
       </c>
@@ -2092,10 +2100,10 @@
       <c r="E2">
         <v>4</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="11">
         <v>7942</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="11">
         <v>7962</v>
       </c>
       <c r="L2" t="s">
@@ -2109,7 +2117,7 @@
       <c r="B3">
         <v>212</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <f t="shared" ref="C3:C10" si="0">A3/B3</f>
         <v>1.5094339622641511</v>
       </c>
@@ -2119,10 +2127,10 @@
       <c r="E3">
         <v>12</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="11">
         <v>7970</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="11">
         <v>7971</v>
       </c>
       <c r="L3" t="s">
@@ -2136,7 +2144,7 @@
       <c r="B4">
         <v>212</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <f t="shared" si="0"/>
         <v>1.5094339622641511</v>
       </c>
@@ -2146,10 +2154,10 @@
       <c r="E4">
         <v>16</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="11">
         <v>7945</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="11">
         <v>7965</v>
       </c>
       <c r="L4" t="s">
@@ -2163,7 +2171,7 @@
       <c r="B5">
         <v>216</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <f t="shared" si="0"/>
         <v>1.4814814814814814</v>
       </c>
@@ -2173,7 +2181,7 @@
       <c r="E5">
         <v>16</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="11">
         <v>7975</v>
       </c>
       <c r="L5" t="s">
@@ -2187,7 +2195,7 @@
       <c r="B6">
         <v>480</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
@@ -2197,19 +2205,19 @@
       <c r="E6">
         <v>24</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="11">
         <v>8941</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="11">
         <v>8945</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="11">
         <v>8961</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="11">
         <v>9951</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="11">
         <v>9971</v>
       </c>
       <c r="L6" t="s">
@@ -2223,7 +2231,7 @@
       <c r="B7">
         <v>600</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
@@ -2233,7 +2241,7 @@
       <c r="E7">
         <v>16</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="11">
         <v>7985</v>
       </c>
       <c r="L7" t="s">
@@ -2247,7 +2255,7 @@
       <c r="B8">
         <v>480</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
@@ -2257,16 +2265,16 @@
       <c r="E8">
         <v>24</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="11">
         <v>8811</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="11">
         <v>8841</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="11">
         <v>8851</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="11">
         <v>8861</v>
       </c>
       <c r="L8" t="s">
@@ -2280,7 +2288,7 @@
       <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>2.7941176470588234</v>
       </c>
@@ -2290,10 +2298,10 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="11">
         <v>7906</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="11">
         <v>7911</v>
       </c>
       <c r="L9" t="s">
@@ -2307,7 +2315,7 @@
       <c r="B10">
         <v>2448</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
@@ -2332,477 +2340,477 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="11">
         <v>7906</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="11">
         <v>369</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="G14" s="10" t="str">
-        <f>C14&amp;" =&gt; {model =&gt;'"&amp;B14&amp;"', res =&gt;'"&amp;D14&amp;"'},"</f>
+      <c r="G14" s="8" t="str">
+        <f t="shared" ref="G14:G32" si="1">C14&amp;" =&gt; {model =&gt;'"&amp;B14&amp;"', res =&gt;'"&amp;D14&amp;"'},"</f>
         <v>369 =&gt; {model =&gt;'7906', res =&gt;'95x34x1'},</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="L14" s="11" t="str">
-        <f>"| "&amp;B14&amp; "|| "&amp; C14&amp;" || &lt;tt&gt;"&amp;D14&amp;"&lt;/tt&gt;"</f>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="L14" s="9" t="str">
+        <f t="shared" ref="L14:L32" si="2">"| "&amp;B14&amp; "|| "&amp; C14&amp;" || &lt;tt&gt;"&amp;D14&amp;"&lt;/tt&gt;"</f>
         <v>| 7906|| 369 || &lt;tt&gt;95x34x1&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="11">
         <v>7911</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="11">
         <v>307</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="G15" s="10" t="str">
-        <f>C15&amp;" =&gt; {model =&gt;'"&amp;B15&amp;"', res =&gt;'"&amp;D15&amp;"'},"</f>
+      <c r="G15" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>307 =&gt; {model =&gt;'7911', res =&gt;'95x34x1'},</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="L15" s="11" t="str">
-        <f>"| "&amp;B15&amp; "|| "&amp; C15&amp;" || &lt;tt&gt;"&amp;D15&amp;"&lt;/tt&gt;"</f>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="L15" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 7911|| 307 || &lt;tt&gt;95x34x1&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B16" s="11">
         <v>7942</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="11">
         <v>434</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="G16" s="10" t="str">
-        <f>C16&amp;" =&gt; {model =&gt;'"&amp;B16&amp;"', res =&gt;'"&amp;D16&amp;"'},"</f>
+      <c r="G16" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>434 =&gt; {model =&gt;'7942', res =&gt;'320x196x4'},</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="L16" s="11" t="str">
-        <f>"| "&amp;B16&amp; "|| "&amp; C16&amp;" || &lt;tt&gt;"&amp;D16&amp;"&lt;/tt&gt;"</f>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="L16" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 7942|| 434 || &lt;tt&gt;320x196x4&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="B17" s="11">
+        <v>7962</v>
+      </c>
+      <c r="C17" s="11">
+        <v>404</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="G17" s="8" t="str">
+        <f>C17&amp;" =&gt; {model =&gt;'"&amp;B17&amp;"', res =&gt;'"&amp;D17&amp;"'},"</f>
+        <v>404 =&gt; {model =&gt;'7962', res =&gt;'320x196x4'},</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="L17" s="9" t="str">
+        <f>"| "&amp;B17&amp; "|| "&amp; C17&amp;" || &lt;tt&gt;"&amp;D17&amp;"&lt;/tt&gt;"</f>
+        <v>| 7962|| 404 || &lt;tt&gt;320x196x4&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
         <v>7945</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="11">
         <v>435</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="G17" s="10" t="str">
-        <f>C17&amp;" =&gt; {model =&gt;'"&amp;B17&amp;"', res =&gt;'"&amp;D17&amp;"'},"</f>
+      <c r="G18" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>435 =&gt; {model =&gt;'7945', res =&gt;'320x212x16'},</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="L17" s="11" t="str">
-        <f>"| "&amp;B17&amp; "|| "&amp; C17&amp;" || &lt;tt&gt;"&amp;D17&amp;"&lt;/tt&gt;"</f>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="L18" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 7945|| 435 || &lt;tt&gt;320x212x16&lt;/tt&gt;</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>7962</v>
-      </c>
-      <c r="C18">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
+        <v>7965</v>
+      </c>
+      <c r="C19" s="11">
+        <v>436</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="G19" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>436 =&gt; {model =&gt;'7965', res =&gt;'320x212x16'},</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="L19" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7965|| 436 || &lt;tt&gt;320x212x16&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
+        <v>7970</v>
+      </c>
+      <c r="C20" s="11">
+        <v>30006</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="G20" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>30006 =&gt; {model =&gt;'7970', res =&gt;'320x212x12'},</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="L20" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7970|| 30006 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <v>7971</v>
+      </c>
+      <c r="C21" s="11">
+        <v>119</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="G21" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>119 =&gt; {model =&gt;'7971', res =&gt;'320x212x12'},</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="L21" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>| 7971|| 119 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
+        <v>7975</v>
+      </c>
+      <c r="C22" s="11">
+        <v>437</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="D18" t="s">
-        <v>402</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="E22" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="G18" s="10" t="str">
-        <f>C18&amp;" =&gt; {model =&gt;'"&amp;B18&amp;"', res =&gt;'"&amp;D18&amp;"'},"</f>
-        <v>404 =&gt; {model =&gt;'7962', res =&gt;'320x212x16'},</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="L18" s="11" t="str">
-        <f>"| "&amp;B18&amp; "|| "&amp; C18&amp;" || &lt;tt&gt;"&amp;D18&amp;"&lt;/tt&gt;"</f>
-        <v>| 7962|| 404 || &lt;tt&gt;320x212x16&lt;/tt&gt;</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>7965</v>
-      </c>
-      <c r="C19">
-        <v>436</v>
-      </c>
-      <c r="D19" t="s">
-        <v>401</v>
-      </c>
-      <c r="E19" t="s">
-        <v>410</v>
-      </c>
-      <c r="G19" s="10" t="str">
-        <f>C19&amp;" =&gt; {model =&gt;'"&amp;B19&amp;"', res =&gt;'"&amp;D19&amp;"'},"</f>
-        <v>436 =&gt; {model =&gt;'7965', res =&gt;'320x196x4'},</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="L19" s="11" t="str">
-        <f>"| "&amp;B19&amp; "|| "&amp; C19&amp;" || &lt;tt&gt;"&amp;D19&amp;"&lt;/tt&gt;"</f>
-        <v>| 7965|| 436 || &lt;tt&gt;320x196x4&lt;/tt&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>7970</v>
-      </c>
-      <c r="C20">
-        <v>30006</v>
-      </c>
-      <c r="D20" t="s">
-        <v>403</v>
-      </c>
-      <c r="E20" t="s">
-        <v>410</v>
-      </c>
-      <c r="G20" s="10" t="str">
-        <f>C20&amp;" =&gt; {model =&gt;'"&amp;B20&amp;"', res =&gt;'"&amp;D20&amp;"'},"</f>
-        <v>30006 =&gt; {model =&gt;'7970', res =&gt;'320x212x12'},</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="L20" s="11" t="str">
-        <f>"| "&amp;B20&amp; "|| "&amp; C20&amp;" || &lt;tt&gt;"&amp;D20&amp;"&lt;/tt&gt;"</f>
-        <v>| 7970|| 30006 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>7971</v>
-      </c>
-      <c r="C21">
-        <v>119</v>
-      </c>
-      <c r="D21" t="s">
-        <v>403</v>
-      </c>
-      <c r="E21" t="s">
-        <v>410</v>
-      </c>
-      <c r="G21" s="10" t="str">
-        <f>C21&amp;" =&gt; {model =&gt;'"&amp;B21&amp;"', res =&gt;'"&amp;D21&amp;"'},"</f>
-        <v>119 =&gt; {model =&gt;'7971', res =&gt;'320x212x12'},</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="L21" s="11" t="str">
-        <f>"| "&amp;B21&amp; "|| "&amp; C21&amp;" || &lt;tt&gt;"&amp;D21&amp;"&lt;/tt&gt;"</f>
-        <v>| 7971|| 119 || &lt;tt&gt;320x212x12&lt;/tt&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>7975</v>
-      </c>
-      <c r="C22">
-        <v>437</v>
-      </c>
-      <c r="D22" t="s">
-        <v>404</v>
-      </c>
-      <c r="E22" t="s">
-        <v>410</v>
-      </c>
-      <c r="G22" s="10" t="str">
-        <f>C22&amp;" =&gt; {model =&gt;'"&amp;B22&amp;"', res =&gt;'"&amp;D22&amp;"'},"</f>
+      <c r="G22" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>437 =&gt; {model =&gt;'7975', res =&gt;'320x216x16'},</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="L22" s="11" t="str">
-        <f>"| "&amp;B22&amp; "|| "&amp; C22&amp;" || &lt;tt&gt;"&amp;D22&amp;"&lt;/tt&gt;"</f>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="L22" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 7975|| 437 || &lt;tt&gt;320x216x16&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="B23" s="11">
         <v>7985</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="11">
         <v>302</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="G23" s="10" t="str">
-        <f>C23&amp;" =&gt; {model =&gt;'"&amp;B23&amp;"', res =&gt;'"&amp;D23&amp;"'},"</f>
+      <c r="G23" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>302 =&gt; {model =&gt;'7985', res =&gt;'800x600x16'},</v>
       </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="L23" s="11" t="str">
-        <f>"| "&amp;B23&amp; "|| "&amp; C23&amp;" || &lt;tt&gt;"&amp;D23&amp;"&lt;/tt&gt;"</f>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="L23" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 7985|| 302 || &lt;tt&gt;800x600x16&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="B24" s="11">
         <v>8811</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="11">
         <v>36217</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="G24" s="10" t="str">
-        <f>C24&amp;" =&gt; {model =&gt;'"&amp;B24&amp;"', res =&gt;'"&amp;D24&amp;"'},"</f>
+      <c r="G24" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>36217 =&gt; {model =&gt;'8811', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="L24" s="11" t="str">
-        <f>"| "&amp;B24&amp; "|| "&amp; C24&amp;" || &lt;tt&gt;"&amp;D24&amp;"&lt;/tt&gt;"</f>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="L24" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 8811|| 36217 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="B25" s="11">
         <v>8841</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="11">
         <v>683</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="G25" s="10" t="str">
-        <f>C25&amp;" =&gt; {model =&gt;'"&amp;B25&amp;"', res =&gt;'"&amp;D25&amp;"'},"</f>
+      <c r="G25" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>683 =&gt; {model =&gt;'8841', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="L25" s="11" t="str">
-        <f>"| "&amp;B25&amp; "|| "&amp; C25&amp;" || &lt;tt&gt;"&amp;D25&amp;"&lt;/tt&gt;"</f>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="L25" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 8841|| 683 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="B26" s="11">
         <v>8851</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="11">
         <v>684</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="G26" s="10" t="str">
-        <f>C26&amp;" =&gt; {model =&gt;'"&amp;B26&amp;"', res =&gt;'"&amp;D26&amp;"'},"</f>
+      <c r="G26" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>684 =&gt; {model =&gt;'8851', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="L26" s="11" t="str">
-        <f>"| "&amp;B26&amp; "|| "&amp; C26&amp;" || &lt;tt&gt;"&amp;D26&amp;"&lt;/tt&gt;"</f>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="L26" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 8851|| 684 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="B27" s="11">
         <v>8861</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="11">
         <v>685</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="G27" s="10" t="str">
-        <f>C27&amp;" =&gt; {model =&gt;'"&amp;B27&amp;"', res =&gt;'"&amp;D27&amp;"'},"</f>
+      <c r="G27" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>685 =&gt; {model =&gt;'8861', res =&gt;'800x480x24'},</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="L27" s="11" t="str">
-        <f>"| "&amp;B27&amp; "|| "&amp; C27&amp;" || &lt;tt&gt;"&amp;D27&amp;"&lt;/tt&gt;"</f>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="L27" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 8861|| 685 || &lt;tt&gt;800x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="B28" s="11">
         <v>8941</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="11">
         <v>586</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="G28" s="10" t="str">
-        <f>C28&amp;" =&gt; {model =&gt;'"&amp;B28&amp;"', res =&gt;'"&amp;D28&amp;"'},"</f>
+      <c r="G28" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>586 =&gt; {model =&gt;'8941', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="L28" s="11" t="str">
-        <f>"| "&amp;B28&amp; "|| "&amp; C28&amp;" || &lt;tt&gt;"&amp;D28&amp;"&lt;/tt&gt;"</f>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="L28" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 8941|| 586 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29">
+      <c r="B29" s="11">
         <v>8945</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="11">
         <v>585</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="G29" s="10" t="str">
-        <f>C29&amp;" =&gt; {model =&gt;'"&amp;B29&amp;"', res =&gt;'"&amp;D29&amp;"'},"</f>
+      <c r="G29" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>585 =&gt; {model =&gt;'8945', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="L29" s="11" t="str">
-        <f>"| "&amp;B29&amp; "|| "&amp; C29&amp;" || &lt;tt&gt;"&amp;D29&amp;"&lt;/tt&gt;"</f>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="L29" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 8945|| 585 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30">
+      <c r="B30" s="11">
         <v>8961</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="11">
         <v>540</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="G30" s="10" t="str">
-        <f>C30&amp;" =&gt; {model =&gt;'"&amp;B30&amp;"', res =&gt;'"&amp;D30&amp;"'},"</f>
+      <c r="G30" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>540 =&gt; {model =&gt;'8961', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="L30" s="11" t="str">
-        <f>"| "&amp;B30&amp; "|| "&amp; C30&amp;" || &lt;tt&gt;"&amp;D30&amp;"&lt;/tt&gt;"</f>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="L30" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 8961|| 540 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31">
+      <c r="B31" s="11">
         <v>9951</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="11">
         <v>537</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="G31" s="10" t="str">
-        <f>C31&amp;" =&gt; {model =&gt;'"&amp;B31&amp;"', res =&gt;'"&amp;D31&amp;"'},"</f>
+      <c r="G31" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>537 =&gt; {model =&gt;'9951', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="L31" s="11" t="str">
-        <f>"| "&amp;B31&amp; "|| "&amp; C31&amp;" || &lt;tt&gt;"&amp;D31&amp;"&lt;/tt&gt;"</f>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="L31" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 9951|| 537 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32">
+      <c r="B32" s="11">
         <v>9971</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="11">
         <v>493</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="G32" s="10" t="str">
-        <f>C32&amp;" =&gt; {model =&gt;'"&amp;B32&amp;"', res =&gt;'"&amp;D32&amp;"'},"</f>
+      <c r="G32" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>493 =&gt; {model =&gt;'9971', res =&gt;'640x480x24'},</v>
       </c>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="L32" s="11" t="str">
-        <f>"| "&amp;B32&amp; "|| "&amp; C32&amp;" || &lt;tt&gt;"&amp;D32&amp;"&lt;/tt&gt;"</f>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="L32" s="9" t="str">
+        <f t="shared" si="2"/>
         <v>| 9971|| 493 || &lt;tt&gt;640x480x24&lt;/tt&gt;</v>
       </c>
     </row>

</xml_diff>